<commit_message>
updeted files with matching names; function to verify all of the names match in both lists and prints a message
</commit_message>
<xml_diff>
--- a/medicaid_data_200.xlsx
+++ b/medicaid_data_200.xlsx
@@ -457,4001 +457,4001 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>916791519</v>
+        <v>91172025</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Brian Clark</t>
+          <t>Samuel Martinez</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2019-04-16</t>
+          <t>2015-11-09</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>David Colon</t>
+          <t>Debra Keller</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>207132705</v>
+        <v>708058959</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Connor Wade</t>
+          <t>Megan Caldwell</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2022-06-09</t>
+          <t>2011-05-15</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Benjamin Sanchez</t>
+          <t>Jordan Arnold</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>297768954</v>
+        <v>929781923</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Christopher King</t>
+          <t>Susan Morton</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2015-01-18</t>
+          <t>2023-10-18</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Zachary Phillips</t>
+          <t>Shawn Wright</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>197037266</v>
+        <v>35642925</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Brittany Brooks</t>
+          <t>Sherri Meyer</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2012-10-08</t>
+          <t>2007-11-03</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Michele Kirk</t>
+          <t>Alicia Rubio</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>44423321</v>
+        <v>100827277</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Anthony Perez</t>
+          <t>Douglas Moses</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2012-01-03</t>
+          <t>2020-11-02</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Robin Hill</t>
+          <t>Luis Watkins</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>71216864</v>
+        <v>566139361</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Christopher Ibarra</t>
+          <t>John West</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2020-12-03</t>
+          <t>2019-10-01</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Robert Gonzalez</t>
+          <t>James Woodward</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>360270679</v>
+        <v>694684760</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Erin Baker</t>
+          <t>Steven Holmes</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2020-02-04</t>
+          <t>2011-08-09</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Jessica Moore</t>
+          <t>Ryan Davis</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>889214644</v>
+        <v>939602152</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Clayton Robertson</t>
+          <t>Joanne Malone</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2011-11-03</t>
+          <t>2008-03-01</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Dennis Smith</t>
+          <t>Heather Harper</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>275123147</v>
+        <v>586605407</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Jacqueline Snyder</t>
+          <t>Danielle Johnson</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2023-02-02</t>
+          <t>2012-05-27</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>William Nelson</t>
+          <t>Stacy Obrien</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>229248382</v>
+        <v>777018863</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Felicia Mcconnell</t>
+          <t>Anthony Weeks</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2014-01-16</t>
+          <t>2016-06-04</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Darren Campbell</t>
+          <t>Donald Schneider</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>204350650</v>
+        <v>30503140</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Bradley Hart</t>
+          <t>Philip Fuller</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2013-06-11</t>
+          <t>2012-02-24</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Thomas Fernandez</t>
+          <t>Pamela Oliver</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>234072033</v>
+        <v>944680570</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Mark Reyes</t>
+          <t>Ronald Hawkins</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2014-08-14</t>
+          <t>2016-02-17</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>James Gillespie</t>
+          <t>Michael Schmidt</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>592975517</v>
+        <v>377986859</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Erica Schaefer</t>
+          <t>Raymond Wheeler</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2011-11-21</t>
+          <t>2023-02-09</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Janet Mitchell</t>
+          <t>Edward Thomas</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>315024417</v>
+        <v>145878623</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Andrew Taylor</t>
+          <t>Brandon West</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2009-06-24</t>
+          <t>2013-11-20</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Kyle Brown</t>
+          <t>Amy Frost</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>360129326</v>
+        <v>256348014</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Karen Pineda</t>
+          <t>Vincent Davis</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2010-12-19</t>
+          <t>2008-01-22</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Richard Brooks</t>
+          <t>Lisa Garrett</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>929192783</v>
+        <v>389083289</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Lauren Holloway</t>
+          <t>Nicholas Rodriguez</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2016-04-25</t>
+          <t>2014-09-13</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Edward Harper</t>
+          <t>James Austin</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>865998691</v>
+        <v>660327770</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Kirk Martinez</t>
+          <t>Paul Jenkins</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2012-11-06</t>
+          <t>2020-05-31</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Amber Hamilton</t>
+          <t>Teresa Jones</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>75659321</v>
+        <v>95046442</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Laurie Lopez</t>
+          <t>Alexandra Diaz</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2009-09-28</t>
+          <t>2007-01-18</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Karen Morgan</t>
+          <t>Shelly Carr</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>265350342</v>
+        <v>708015865</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Jessica Young</t>
+          <t>Kevin Brown</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2010-11-19</t>
+          <t>2010-08-18</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Julie Jones</t>
+          <t>Sharon Allen</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>420499083</v>
+        <v>584269705</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Sue Parker</t>
+          <t>Ronald Miller</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2006-07-01</t>
+          <t>2016-11-11</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Marc Garcia</t>
+          <t>Steven Brown</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>571135230</v>
+        <v>181350998</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Juan Blackburn</t>
+          <t>Bradley Scott</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2006-06-04</t>
+          <t>2015-04-28</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Randall Thompson</t>
+          <t>Justin Anderson</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>113584840</v>
+        <v>217879659</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Jeffrey Aguirre</t>
+          <t>Jessica Hamilton</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2009-11-25</t>
+          <t>2008-08-10</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Angela Bowman</t>
+          <t>Michael Bullock</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>920951803</v>
+        <v>724705693</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Bryan Aguilar</t>
+          <t>Sandra Russell</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2016-10-25</t>
+          <t>2016-07-06</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Richard Young</t>
+          <t>Meghan Butler</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>327485463</v>
+        <v>502841362</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Anne Stevenson</t>
+          <t>Heather Duffy</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2009-09-10</t>
+          <t>2019-04-30</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>John Hobbs</t>
+          <t>Joanna Hopkins</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>718485885</v>
+        <v>75535677</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Kristen Frost</t>
+          <t>Steven Walker</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2024-05-21</t>
+          <t>2015-08-24</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Sheila Chambers</t>
+          <t>Heather Brooks</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>65019185</v>
+        <v>753484277</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Maurice Mitchell</t>
+          <t>Jacqueline Conner</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2020-02-09</t>
+          <t>2010-10-02</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Danielle Greene</t>
+          <t>Eric Skinner</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>457707139</v>
+        <v>897294334</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Courtney Garcia</t>
+          <t>Jeffery Adams</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2010-11-19</t>
+          <t>2017-01-25</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Matthew Brown</t>
+          <t>John Carter</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>509456244</v>
+        <v>495077686</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Ryan Mckenzie</t>
+          <t>Donna Lee</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2008-01-02</t>
+          <t>2008-04-27</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Kristopher Harris</t>
+          <t>John Snyder</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>111380521</v>
+        <v>92590838</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Melissa Hubbard</t>
+          <t>Nicole Butler</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2019-10-23</t>
+          <t>2014-08-30</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Jeremy Drake</t>
+          <t>Deborah Price</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>10389105</v>
+        <v>525861589</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Victoria Daugherty</t>
+          <t>John Morris</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2012-08-31</t>
+          <t>2018-10-24</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>John Lucas</t>
+          <t>Kathy Woodward</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>581798114</v>
+        <v>802295223</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Marisa Stephens</t>
+          <t>William Daniel</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2013-03-07</t>
+          <t>2023-02-05</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Austin Wiggins</t>
+          <t>Natalie Casey</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>293105993</v>
+        <v>812737586</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Lori Allen</t>
+          <t>Michael Zimmerman</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2018-06-28</t>
+          <t>2015-01-14</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Thomas Hampton</t>
+          <t>Roger Martin</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>783618426</v>
+        <v>530281782</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Tiffany Mercado</t>
+          <t>David White</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2022-05-10</t>
+          <t>2006-10-30</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Janice Lopez</t>
+          <t>Daisy Jackson</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>134558104</v>
+        <v>759094117</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Brett Cain</t>
+          <t>Yolanda Browning</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2018-01-15</t>
+          <t>2016-08-07</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Tyler Acosta</t>
+          <t>Kelly Wells</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>774308150</v>
+        <v>226599524</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Laura Booth</t>
+          <t>Jeffery Larson</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2006-09-17</t>
+          <t>2011-06-22</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Jesus Banks</t>
+          <t>Victoria Sullivan</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>575055597</v>
+        <v>126596785</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Anthony Brown</t>
+          <t>Nicolas Riley</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2006-04-09</t>
+          <t>2014-09-05</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Charles Cantu</t>
+          <t>Eric Tanner</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>149803556</v>
+        <v>774235143</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Jeffrey Willis</t>
+          <t>Elizabeth Hanson</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2007-09-15</t>
+          <t>2021-07-28</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Kristi Aguilar</t>
+          <t>Lisa Williams</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>805582207</v>
+        <v>640904014</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Chad Wilson</t>
+          <t>Diana Lowe</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2013-06-11</t>
+          <t>2009-07-30</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Michael Cole</t>
+          <t>Tina Hopkins</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>819272002</v>
+        <v>892681313</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Nicholas Becker</t>
+          <t>Gina Jones</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2013-11-07</t>
+          <t>2011-06-11</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Debbie Wood</t>
+          <t>Stephanie Garza</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>841265555</v>
+        <v>215786223</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Zachary Knox</t>
+          <t>Leslie Tucker</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2006-02-28</t>
+          <t>2010-04-04</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Jennifer Davis</t>
+          <t>Ryan Cox</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>979394862</v>
+        <v>53653843</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Lori Mccarty</t>
+          <t>Nathaniel Johnson</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2021-11-28</t>
+          <t>2018-05-30</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Dennis Miller</t>
+          <t>Virginia Hodges</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>56194793</v>
+        <v>246349099</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Shelia Owens</t>
+          <t>Johnny Gutierrez</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2011-07-09</t>
+          <t>2021-04-25</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>James Black</t>
+          <t>Stephanie Gordon</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>284246546</v>
+        <v>907178779</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Jennifer Walter</t>
+          <t>Allison Brooks</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2023-02-26</t>
+          <t>2006-12-12</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Jeremy Mcintosh</t>
+          <t>Wendy Bradley</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>941979920</v>
+        <v>873481223</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Steven Hamilton</t>
+          <t>Brandon Howard</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2020-10-17</t>
+          <t>2023-12-22</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Martha Strickland</t>
+          <t>Donna Ali</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>162777877</v>
+        <v>88614306</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Gregory Smith</t>
+          <t>Steven Frazier</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2009-09-07</t>
+          <t>2007-01-18</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Roger Carpenter</t>
+          <t>Sarah Cochran</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>230721411</v>
+        <v>826506463</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Denise Nicholson</t>
+          <t>Ronald Kim</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2019-02-28</t>
+          <t>2018-09-14</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Michael Morales</t>
+          <t>Colin Davis</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>808693059</v>
+        <v>856631867</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Tony Nixon</t>
+          <t>Daniel Duran</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2024-06-24</t>
+          <t>2020-05-16</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Jonathan Edwards</t>
+          <t>Michael Bradshaw</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>883193072</v>
+        <v>202546360</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Matthew Scott</t>
+          <t>Julie Thomas</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2017-07-30</t>
+          <t>2021-09-01</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Jill Hogan</t>
+          <t>Mary Clark</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>292453875</v>
+        <v>305052433</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Mark Lloyd</t>
+          <t>Natalie Burke</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2007-11-16</t>
+          <t>2010-04-27</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Megan Marshall</t>
+          <t>Brendan Morales</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>497789577</v>
+        <v>71424730</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Walter Bailey</t>
+          <t>Christopher Ryan</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2010-03-05</t>
+          <t>2021-12-05</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Anthony Burke</t>
+          <t>Christopher Weiss</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>146705990</v>
+        <v>303236670</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Emily Martin</t>
+          <t>Tammy Sawyer</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2021-10-23</t>
+          <t>2020-04-01</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Amanda Daugherty</t>
+          <t>Rhonda Martinez</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>268285069</v>
+        <v>414586832</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Joel Vaughn</t>
+          <t>Sarah Wright</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2010-02-05</t>
+          <t>2022-12-22</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Joshua Singh</t>
+          <t>Jerry George</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>182793226</v>
+        <v>116742385</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Karen Arnold</t>
+          <t>Nancy Thompson</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2006-05-25</t>
+          <t>2010-08-04</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Mia Nguyen</t>
+          <t>Christopher Bush</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>106478915</v>
+        <v>989659244</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Jose Simpson</t>
+          <t>Margaret Navarro</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2010-12-08</t>
+          <t>2019-09-10</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Andrea Cox</t>
+          <t>Christine Graves</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>813208984</v>
+        <v>26476577</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Jennifer Gilbert</t>
+          <t>Cody Johnson</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2023-04-27</t>
+          <t>2008-10-07</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>William Dean</t>
+          <t>Henry Walsh</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>110791912</v>
+        <v>86131103</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Lauren Wilkerson</t>
+          <t>Austin Figueroa</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2006-09-17</t>
+          <t>2019-03-24</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Aaron Chavez</t>
+          <t>Maria Steele</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>336555598</v>
+        <v>707808612</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Kevin Cox</t>
+          <t>Amber Alexander</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2006-10-06</t>
+          <t>2010-08-21</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Mary Roberts</t>
+          <t>Jimmy Anderson</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>297924229</v>
+        <v>55488135</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Austin Porter</t>
+          <t>Sarah Morgan</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2006-10-10</t>
+          <t>2011-05-04</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Maria Rivera</t>
+          <t>Christopher Stewart</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>645631153</v>
+        <v>766901427</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Christopher Blankenship</t>
+          <t>Vincent Wong</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2021-03-03</t>
+          <t>2023-11-06</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Laura Smith</t>
+          <t>Jennifer Luna</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>348837953</v>
+        <v>292769313</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Kristie Murphy</t>
+          <t>Kyle Alvarez</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2014-03-13</t>
+          <t>2012-05-03</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>David Myers</t>
+          <t>Amy Ashley</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>502411173</v>
+        <v>456218353</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Brandon Scott</t>
+          <t>Carrie Sanchez</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2017-05-02</t>
+          <t>2007-08-18</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Debbie Martin</t>
+          <t>Megan Clarke</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>423854804</v>
+        <v>856509226</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>William Gibson</t>
+          <t>Mario Kim</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2018-12-05</t>
+          <t>2010-04-21</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Christine Pham</t>
+          <t>Kathy Edwards</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>675258502</v>
+        <v>368602970</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>John Russell</t>
+          <t>Alexander May</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>2016-01-31</t>
+          <t>2023-12-11</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Andrew Rush</t>
+          <t>Cynthia Barber</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>756377362</v>
+        <v>178412860</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Holly Lopez</t>
+          <t>Jonathon Sullivan</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>2023-08-25</t>
+          <t>2006-09-03</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Jesus Perry</t>
+          <t>Rebecca Weeks</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>54566808</v>
+        <v>409638998</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Sarah Foster</t>
+          <t>Laura Moyer</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>2017-03-01</t>
+          <t>2014-05-27</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Jessica Maxwell</t>
+          <t>Yesenia Williams</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>64836230</v>
+        <v>591450886</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Kevin Chapman</t>
+          <t>Vanessa Cox</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>2012-08-18</t>
+          <t>2020-01-13</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Robin Robinson</t>
+          <t>Ashley Pennington</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>64280100</v>
+        <v>813583184</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Michael Gonzales</t>
+          <t>Amy Carson</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>2016-10-22</t>
+          <t>2019-09-03</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Christopher Becker</t>
+          <t>Chad Davis</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>118571452</v>
+        <v>485488415</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Jade Murillo</t>
+          <t>Michelle Hanson</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>2013-06-30</t>
+          <t>2022-06-07</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Gabriel Mcdonald</t>
+          <t>Rita Robinson</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>389233246</v>
+        <v>918607062</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Jerry Pearson</t>
+          <t>Mark Rogers</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>2007-06-07</t>
+          <t>2023-10-15</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Shannon Kelly</t>
+          <t>Ashley Rhodes</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>631387281</v>
+        <v>365094114</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Gregory Coleman</t>
+          <t>Ruth Luna</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>2019-09-08</t>
+          <t>2010-12-23</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Michelle Allen</t>
+          <t>Tina Woodward</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>610976040</v>
+        <v>778034992</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Marcus Moreno</t>
+          <t>Wayne Kirby</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>2015-12-17</t>
+          <t>2008-01-18</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>William Boyd</t>
+          <t>Joseph Ross</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>409380727</v>
+        <v>205187054</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Derek Houston</t>
+          <t>Julie Nelson</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>2008-12-08</t>
+          <t>2022-03-14</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Mary Lucas</t>
+          <t>Brandy Morgan</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>568509561</v>
+        <v>19683687</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Ryan Wilkins</t>
+          <t>Kayla Holmes</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>2006-07-17</t>
+          <t>2014-08-10</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Christopher Clayton</t>
+          <t>Eric Edwards</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>290756867</v>
+        <v>734387829</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Matthew Thompson</t>
+          <t>Mike Montes</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>2005-10-19</t>
+          <t>2014-03-07</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Michelle Hernandez</t>
+          <t>Joshua Hall</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>139569656</v>
+        <v>775717391</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Rebecca Johnson</t>
+          <t>Nathaniel Palmer</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>2014-08-06</t>
+          <t>2014-06-27</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Jeremy Sanchez</t>
+          <t>Brittany Small</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>823132704</v>
+        <v>96480972</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Danielle Compton</t>
+          <t>Tara Clark</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>2018-01-28</t>
+          <t>2018-08-23</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Michael Brown</t>
+          <t>Christina Mclaughlin</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>843378844</v>
+        <v>412806954</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Deborah Blanchard</t>
+          <t>Samuel Morrow</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>2017-01-13</t>
+          <t>2023-04-21</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Richard Taylor</t>
+          <t>Katherine Wagner</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>848458115</v>
+        <v>701439052</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Thomas Carey</t>
+          <t>Eric Morris</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>2014-04-21</t>
+          <t>2023-07-31</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Joseph Adams</t>
+          <t>Crystal Russell</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>451504974</v>
+        <v>503495199</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Patrick Burns</t>
+          <t>Cindy Curtis</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>2007-11-18</t>
+          <t>2022-06-17</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Eugene Hood</t>
+          <t>Carla Rose</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>232657926</v>
+        <v>444846198</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Angela Dennis</t>
+          <t>Katie Tapia</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>2011-04-11</t>
+          <t>2020-01-13</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Colin Marks</t>
+          <t>Alexis Lopez</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>704814738</v>
+        <v>622783357</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Crystal Wallace</t>
+          <t>Samantha Guzman</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>2018-06-11</t>
+          <t>2006-06-03</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Christopher Reeves</t>
+          <t>Lisa Williams</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>358769578</v>
+        <v>672851163</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Katie Garcia</t>
+          <t>Cole Rodriguez</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>2008-07-09</t>
+          <t>2014-11-05</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Stacy Rivera</t>
+          <t>Jamie Moore</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>862341671</v>
+        <v>424122313</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Tyler Oconnell</t>
+          <t>Shawn Hughes</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>2024-04-13</t>
+          <t>2019-12-07</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Joel Fox</t>
+          <t>Nicole Davis</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>870321526</v>
+        <v>832635110</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Christopher Donovan</t>
+          <t>Mary Cardenas</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>2020-06-06</t>
+          <t>2007-05-06</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Jacob Lee</t>
+          <t>Alan Hahn</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>118884708</v>
+        <v>695078322</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Stacie Burns</t>
+          <t>Cathy Fuller</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>2023-11-24</t>
+          <t>2008-04-08</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Andrea Hansen</t>
+          <t>Frank Schmidt</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>552040844</v>
+        <v>377203317</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Kayla Fischer</t>
+          <t>Keith Lindsey</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>2014-01-11</t>
+          <t>2021-08-14</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Sarah Hall</t>
+          <t>John White</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>620806849</v>
+        <v>280411658</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Bradley Johnson</t>
+          <t>Laura Bass</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>2010-05-14</t>
+          <t>2022-01-08</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Christopher Campos</t>
+          <t>Joseph Morales</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>41996503</v>
+        <v>970543161</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Joshua Wright</t>
+          <t>Alex Buckley</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>2016-10-29</t>
+          <t>2014-07-08</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>David Thornton</t>
+          <t>Richard Anderson</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>321473223</v>
+        <v>515260955</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Robert Fitzpatrick</t>
+          <t>Beth Hood</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>2010-06-11</t>
+          <t>2016-08-17</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Edward Crawford</t>
+          <t>Jeffrey Johnson</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>286105359</v>
+        <v>253304489</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Daniel Palmer</t>
+          <t>Laura Phillips</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>2014-07-10</t>
+          <t>2019-04-03</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Ashley Wheeler</t>
+          <t>Paige Williams</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>687982401</v>
+        <v>436759840</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>April Solomon</t>
+          <t>Craig Murphy</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>2008-09-21</t>
+          <t>2011-01-20</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Jane Smith</t>
+          <t>Trevor Hudson</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>875468006</v>
+        <v>471390898</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Ricky Cunningham</t>
+          <t>Autumn Smith</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>2008-06-17</t>
+          <t>2015-02-12</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Angela Barber</t>
+          <t>Emma Moore</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>950480318</v>
+        <v>633230773</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Kelly Eaton</t>
+          <t>Tyler Bailey</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>2020-03-03</t>
+          <t>2009-07-22</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Haley Cox</t>
+          <t>Stephen Lee</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>671310828</v>
+        <v>379987079</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Brandon Smith</t>
+          <t>Nathan Carter</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>2017-05-11</t>
+          <t>2018-03-11</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Jason Rice</t>
+          <t>Christina Davenport</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>936337253</v>
+        <v>722812959</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Lisa Mendez</t>
+          <t>Briana Jordan</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>2007-08-05</t>
+          <t>2013-12-22</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Robyn Torres</t>
+          <t>Emily Preston</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>201404044</v>
+        <v>297025340</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Joseph Braun</t>
+          <t>Nathaniel Richardson</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>2022-03-15</t>
+          <t>2009-01-25</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Ariana Brown</t>
+          <t>Mark Dennis</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>73149170</v>
+        <v>623315476</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Dillon Cunningham</t>
+          <t>Christine Brown</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>2019-05-19</t>
+          <t>2007-02-05</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Chris Singleton</t>
+          <t>Mary Richardson</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>906038641</v>
+        <v>824128801</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Robin Garcia</t>
+          <t>Stephanie Gutierrez</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>2010-03-26</t>
+          <t>2008-04-09</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Gregory Olsen</t>
+          <t>Kimberly Johnson</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>941839000</v>
+        <v>27396701</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>David Carr</t>
+          <t>Rita Robinson</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>2006-02-06</t>
+          <t>2018-11-01</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Kelly Estrada</t>
+          <t>William Yoder</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>579271143</v>
+        <v>160231641</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Jeremy Sutton</t>
+          <t>Gwendolyn Hudson</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>2019-07-14</t>
+          <t>2023-12-10</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Cindy Woods</t>
+          <t>Derek Taylor</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>685493150</v>
+        <v>647233428</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>John Byrd</t>
+          <t>Melissa Nielsen</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>2010-12-07</t>
+          <t>2006-09-28</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Jennifer Thomas</t>
+          <t>Hailey Sanchez</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>223241592</v>
+        <v>701639748</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Jesse Miller</t>
+          <t>Jonathan Perez</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>2022-02-26</t>
+          <t>2006-03-13</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Taylor Duncan</t>
+          <t>Ryan Ray</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>227617096</v>
+        <v>487304543</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Katie Lopez</t>
+          <t>Brenda Rivera</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>2006-12-25</t>
+          <t>2016-01-20</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Kelly Patterson</t>
+          <t>Nicole Sellers</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>857783254</v>
+        <v>527559316</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>John Dunn</t>
+          <t>Sarah Franklin</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>2007-04-14</t>
+          <t>2008-01-08</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Paul Franklin</t>
+          <t>Fred Cruz</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>539447</v>
+        <v>962044401</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Katie Richards</t>
+          <t>Andrea Benjamin</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>2008-09-02</t>
+          <t>2015-11-14</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Gary Hunter</t>
+          <t>Shawn Harris</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>662694793</v>
+        <v>1719891</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Mary Norris</t>
+          <t>Michael Oliver</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>2009-03-07</t>
+          <t>2022-01-05</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Joshua Adams</t>
+          <t>Lisa May</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>343888059</v>
+        <v>791527918</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Alison Smith</t>
+          <t>Madison Davis</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>2024-06-17</t>
+          <t>2021-03-14</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Jennifer Boone</t>
+          <t>William Murphy</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>978307672</v>
+        <v>427098411</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Jill Vaughn</t>
+          <t>Theresa Velasquez</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>2010-07-21</t>
+          <t>2010-09-16</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Carl Farley</t>
+          <t>Kimberly Rodriguez</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>342472139</v>
+        <v>798980255</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Sergio Snyder</t>
+          <t>Cody Bright</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>2021-01-14</t>
+          <t>2011-07-15</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Kayla Harrington</t>
+          <t>Robert Fields</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>659962831</v>
+        <v>189323905</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Mitchell Nixon</t>
+          <t>Debbie Harris</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>2017-05-30</t>
+          <t>2019-02-16</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Billy Pearson</t>
+          <t>Dalton Carroll</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>578711651</v>
+        <v>1684441</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Ryan Chen</t>
+          <t>Edgar Brown</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>2020-06-20</t>
+          <t>2008-11-29</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Christopher Valentine</t>
+          <t>Lisa White</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>849674486</v>
+        <v>699498402</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Robert Romero</t>
+          <t>Anthony Curtis</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>2014-04-30</t>
+          <t>2007-08-11</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Shannon Gonzalez</t>
+          <t>Tara Salazar</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>552600597</v>
+        <v>80123489</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Patrick Shaw</t>
+          <t>Gregory Allen</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>2005-10-11</t>
+          <t>2017-03-16</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Veronica Gomez</t>
+          <t>Heidi Davis</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>874408198</v>
+        <v>681079585</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>John Miller</t>
+          <t>Darryl Lambert</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>2016-02-12</t>
+          <t>2021-11-04</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Benjamin Miller</t>
+          <t>Brett Jacobs</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>366718363</v>
+        <v>425603003</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Patrick Payne</t>
+          <t>Elizabeth Parker</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>2008-04-13</t>
+          <t>2015-10-15</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Lindsay Stephens</t>
+          <t>Jennifer Olson</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>374174183</v>
+        <v>858760814</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Desiree Duran</t>
+          <t>Dustin West</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>2013-09-19</t>
+          <t>2010-11-16</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Karen Freeman</t>
+          <t>Joanne Walker</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>358196405</v>
+        <v>996226630</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Johnathan Hamilton</t>
+          <t>Matthew Miller</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>2012-09-24</t>
+          <t>2010-09-14</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Kristina Miller</t>
+          <t>Joanne Harris</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>875217086</v>
+        <v>264751370</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Peter Allen</t>
+          <t>Michael Gonzalez</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>2018-01-18</t>
+          <t>2013-03-19</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Lisa Smith</t>
+          <t>Jillian Ramirez</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>210365326</v>
+        <v>293543718</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Daniel Benjamin</t>
+          <t>Heidi Murphy</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>2012-02-19</t>
+          <t>2023-02-22</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Jesse Rivera</t>
+          <t>Lucas Crawford</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>614360486</v>
+        <v>271155178</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Jason Lewis</t>
+          <t>Matthew Garcia</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>2008-04-22</t>
+          <t>2016-01-05</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Daisy Ingram</t>
+          <t>Margaret Norton</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>206705921</v>
+        <v>534284956</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Judy Smith</t>
+          <t>James Dunlap</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>2023-11-13</t>
+          <t>2014-09-09</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Patricia Lewis</t>
+          <t>Brenda Murphy</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>735062042</v>
+        <v>16574034</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Heather Allison</t>
+          <t>Alexander Garcia</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>2012-10-06</t>
+          <t>2012-07-11</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Samantha Roman</t>
+          <t>Anna Campbell</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>765094966</v>
+        <v>495027492</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>James Johnson</t>
+          <t>David Perez</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>2014-10-24</t>
+          <t>2022-04-18</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Michael Day</t>
+          <t>Timothy Reyes</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>825603048</v>
+        <v>55994434</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Crystal Gill</t>
+          <t>Nicole Martin</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>2018-12-17</t>
+          <t>2017-01-18</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Michael Davies</t>
+          <t>Julie Frost</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>543674136</v>
+        <v>690109320</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Elizabeth Hall</t>
+          <t>Christine Brown</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>2021-01-19</t>
+          <t>2006-02-16</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Matthew Sanchez</t>
+          <t>Nancy Dalton</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>124646268</v>
+        <v>907919468</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>William Taylor</t>
+          <t>Wanda Palmer</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>2021-08-23</t>
+          <t>2006-01-12</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Catherine Long</t>
+          <t>Kimberly White</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>323315025</v>
+        <v>9720420</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Jacob Davis</t>
+          <t>Michelle Stewart</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>2017-07-29</t>
+          <t>2017-04-03</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Valerie Park</t>
+          <t>Laurie Flores</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>9781863</v>
+        <v>515077170</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Mary French</t>
+          <t>Samantha Ramirez</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>2022-05-04</t>
+          <t>2006-03-05</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Michelle George</t>
+          <t>Stephanie Jones</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>120101798</v>
+        <v>962114505</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Kelly Lambert</t>
+          <t>Jason Hunter</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>2021-05-31</t>
+          <t>2020-03-27</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Nathaniel Sharp</t>
+          <t>Kim Simon</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>326190371</v>
+        <v>346792530</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Kelsey Foster</t>
+          <t>Todd Martin</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>2024-09-13</t>
+          <t>2018-03-29</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Timothy Gilbert</t>
+          <t>Anthony Holmes</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>124525063</v>
+        <v>472649835</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Christine Armstrong</t>
+          <t>Michael Lee</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>2021-12-13</t>
+          <t>2017-12-22</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>William Jackson</t>
+          <t>Andres Jones</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>246342361</v>
+        <v>536109463</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Tammie Jackson</t>
+          <t>James Mason</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>2007-09-07</t>
+          <t>2006-07-08</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>John James</t>
+          <t>Sandra Jones</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>75769680</v>
+        <v>544608708</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Rodney Golden</t>
+          <t>Alejandro Moore</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>2016-03-08</t>
+          <t>2019-01-17</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Eddie Taylor</t>
+          <t>Fernando Simmons</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>693486145</v>
+        <v>542625123</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Raymond Bryant</t>
+          <t>David Leach</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>2006-12-03</t>
+          <t>2013-03-08</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>Cory Warren</t>
+          <t>Tara Juarez</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>406805070</v>
+        <v>395933372</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Troy James</t>
+          <t>Randy Allen</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>2006-01-11</t>
+          <t>2017-06-20</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Chad Nixon</t>
+          <t>Deborah Foster</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>997206267</v>
+        <v>405461988</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Dylan Scott</t>
+          <t>Edward Washington</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>2012-05-08</t>
+          <t>2020-08-20</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Shawn Moody</t>
+          <t>Frank Brown</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>646759271</v>
+        <v>658557892</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Bobby Brown</t>
+          <t>Cynthia Snyder</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>2008-01-25</t>
+          <t>2005-12-22</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>Paul Perez</t>
+          <t>Laura Johnson</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>288346582</v>
+        <v>606481068</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Robert Baker</t>
+          <t>Anna Larson</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>2008-07-21</t>
+          <t>2020-12-12</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>Jessica Lewis</t>
+          <t>Kimberly Dunn</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>502264959</v>
+        <v>985805746</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Daniel Gilmore</t>
+          <t>Kimberly Adams</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>2010-01-11</t>
+          <t>2023-01-18</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>Jared Mcneil</t>
+          <t>Mark Mclean</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>900268027</v>
+        <v>922798511</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Debbie Pierce</t>
+          <t>Amanda Scott</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>2016-08-30</t>
+          <t>2015-09-18</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>Gene Kelly</t>
+          <t>Karen Gallagher</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>253075302</v>
+        <v>60736143</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Michelle Johnson</t>
+          <t>Mary Perez</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>2017-12-20</t>
+          <t>2011-10-12</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>Peter Collins</t>
+          <t>Kristina Swanson</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>396889426</v>
+        <v>552922789</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>George Wright</t>
+          <t>Christopher Wallace</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>2007-11-14</t>
+          <t>2021-08-06</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>Danielle Wade</t>
+          <t>Katherine Weber</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>384504638</v>
+        <v>897632169</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Susan Turner</t>
+          <t>Kathleen Clarke</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>2007-05-18</t>
+          <t>2016-12-12</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>Tony Church</t>
+          <t>Julia Jensen</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>292961923</v>
+        <v>11247059</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Michael Williams</t>
+          <t>Rebecca Allison</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>2015-04-22</t>
+          <t>2013-06-23</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>Felicia Wilson</t>
+          <t>Erica Russo</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>404675849</v>
+        <v>560131104</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Harold Nguyen</t>
+          <t>Alexa Wilson</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>2008-12-27</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>Nathaniel Thompson</t>
+          <t>Natalie Collins</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>326358002</v>
+        <v>517332356</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Eric Dickerson</t>
+          <t>Daniel Ramirez</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>2024-02-26</t>
+          <t>2005-10-09</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>Thomas Lowe</t>
+          <t>Gabrielle Perry</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>702189989</v>
+        <v>631917094</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Loretta Rodgers</t>
+          <t>Erik Jordan</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>2019-04-25</t>
+          <t>2020-06-18</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>Cassandra Harrison</t>
+          <t>Daniel Haynes</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>714144048</v>
+        <v>15412816</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Beth Hogan</t>
+          <t>Patrick Schwartz</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>2018-05-27</t>
+          <t>2008-09-15</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>Erin Gordon</t>
+          <t>Emily Hill</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>997637584</v>
+        <v>339656306</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>William Weber</t>
+          <t>Annette Chung</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>2012-02-17</t>
+          <t>2021-05-27</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>Michael Brown</t>
+          <t>Brandi Walker</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>971606466</v>
+        <v>999553031</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Holly Riley</t>
+          <t>Matthew Crawford</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>2015-09-10</t>
+          <t>2008-11-12</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>Cindy Walsh</t>
+          <t>Edward Petersen</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>675021605</v>
+        <v>553808200</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Toni Thompson</t>
+          <t>Shari Mclaughlin</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>2022-10-08</t>
+          <t>2021-02-20</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>Jillian Anderson</t>
+          <t>Shawn Ruiz</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>261314024</v>
+        <v>93426098</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>John Hall</t>
+          <t>Justin Rojas</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>2020-08-27</t>
+          <t>2020-11-21</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>Christina Aguilar</t>
+          <t>Linda Smith</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>807552598</v>
+        <v>795844325</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Alexandra Drake</t>
+          <t>Susan Tucker</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>2009-08-01</t>
+          <t>2022-09-04</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>Angela Stewart</t>
+          <t>Connie Henderson</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>396815621</v>
+        <v>956490754</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Elizabeth Mann</t>
+          <t>Paul Le</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>2018-06-24</t>
+          <t>2017-06-08</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>Barbara Nelson</t>
+          <t>Robin Mitchell</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>297666439</v>
+        <v>577311719</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Nicholas Johnson</t>
+          <t>Michael Smith</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>2011-12-22</t>
+          <t>2011-08-13</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>Nathan Murphy</t>
+          <t>Megan Cordova</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>202721515</v>
+        <v>379638736</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Samantha Kent</t>
+          <t>Darrell Thompson</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>2005-12-25</t>
+          <t>2014-08-15</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>Caleb Burns</t>
+          <t>Bob Hughes</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>666859583</v>
+        <v>620787622</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Megan Mack</t>
+          <t>Jessica Allen</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>2014-05-20</t>
+          <t>2010-07-15</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>Anthony Montgomery</t>
+          <t>Adrian Schroeder</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>327610004</v>
+        <v>363896109</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Lisa Smith</t>
+          <t>John Washington</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>2007-07-06</t>
+          <t>2015-07-29</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>Michael Owens</t>
+          <t>Brian Friedman</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>955021004</v>
+        <v>798844345</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Timothy Ellis</t>
+          <t>Adam Ford</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>2008-05-16</t>
+          <t>2012-06-25</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>Jimmy Griffith</t>
+          <t>Kimberly Contreras</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>343767627</v>
+        <v>996624136</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Victoria Cox</t>
+          <t>Amanda Sexton</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>2015-12-09</t>
+          <t>2019-12-06</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>David Torres</t>
+          <t>Brian Franco</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>964547703</v>
+        <v>70538068</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Courtney Sandoval</t>
+          <t>Rick Hughes</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>2008-12-02</t>
+          <t>2024-01-02</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>Thomas Cox</t>
+          <t>Eric David</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>317545819</v>
+        <v>476993040</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Donald Adams</t>
+          <t>Jennifer Jennings</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>2022-10-18</t>
+          <t>2017-06-24</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>John Ward</t>
+          <t>Amanda Park</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>630536490</v>
+        <v>343813330</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Kayla Ray</t>
+          <t>Jeffrey Sutton</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>2022-12-04</t>
+          <t>2013-11-08</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>Bethany Romero</t>
+          <t>Adam Williams</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>152363451</v>
+        <v>457227780</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Daniel Jackson</t>
+          <t>Melissa Oliver</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>2013-03-17</t>
+          <t>2019-04-12</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>Russell Scott</t>
+          <t>Ashley Rhodes</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>937889999</v>
+        <v>656294080</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Patricia Snow</t>
+          <t>Vicki English</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>2016-04-11</t>
+          <t>2020-01-10</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>Melanie Smith</t>
+          <t>Michele Lozano</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>59486135</v>
+        <v>27553992</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Holly Meyers</t>
+          <t>John Rivera</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>2022-06-20</t>
+          <t>2013-06-09</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>Kathleen Jones</t>
+          <t>Leslie Baker</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>298604155</v>
+        <v>423642409</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Ryan Camacho</t>
+          <t>Elizabeth Parker</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>2013-08-14</t>
+          <t>2009-01-26</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>Kristy Roberts</t>
+          <t>Jennifer Smith</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>468710181</v>
+        <v>986542413</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Sarah Olson</t>
+          <t>Sonia Parker</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>2018-12-06</t>
+          <t>2008-09-22</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>Donna Gay</t>
+          <t>Carol Sullivan</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>516058911</v>
+        <v>227017396</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Tracey Herrera</t>
+          <t>Zachary Moody</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>2010-05-25</t>
+          <t>2019-10-12</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>Ashlee Taylor</t>
+          <t>Robert Caldwell</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>862230928</v>
+        <v>682886608</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Catherine Bean</t>
+          <t>Suzanne Smith</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>2016-03-20</t>
+          <t>2019-04-01</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>Samantha Rivera</t>
+          <t>Robert Simmons</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>352969517</v>
+        <v>32017595</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Chelsea Jensen</t>
+          <t>Scott Miller</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>2019-06-04</t>
+          <t>2024-03-18</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>Elizabeth Davis</t>
+          <t>Heather Larson</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>910746178</v>
+        <v>953659007</v>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Andrew Taylor</t>
+          <t>Jamie Gardner</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>2021-02-15</t>
+          <t>2008-05-04</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>Charles Turner</t>
+          <t>Alice Barnes</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>958053446</v>
+        <v>579814617</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Regina Kelly</t>
+          <t>Marisa Brooks</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>2016-07-19</t>
+          <t>2007-04-26</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>Jessica Lowery</t>
+          <t>Joshua Jones</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>535551438</v>
+        <v>410189739</v>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Michelle Guerra</t>
+          <t>Jessica Boone</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>2024-07-12</t>
+          <t>2007-10-18</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>Christopher Rivera</t>
+          <t>Walter Young</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>214562311</v>
+        <v>596131268</v>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Renee Scott</t>
+          <t>Ashley Glass</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>2019-11-11</t>
+          <t>2009-06-04</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>Jennifer Vasquez</t>
+          <t>Debra Powell</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>883121826</v>
+        <v>208740321</v>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Robert Mcdonald</t>
+          <t>Cristian Waters</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>2011-11-26</t>
+          <t>2020-03-12</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>Kelsey Hansen</t>
+          <t>Austin Barnes</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>871935843</v>
+        <v>606047395</v>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Katherine Anderson</t>
+          <t>Justin Robbins</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>2012-01-06</t>
+          <t>2017-10-13</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>Wendy Ramos</t>
+          <t>Jennifer Lee</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>175166122</v>
+        <v>128691423</v>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Mariah Rodriguez</t>
+          <t>Crystal Yang</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>2013-02-27</t>
+          <t>2012-01-24</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>James Alexander</t>
+          <t>Daniel Fisher</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>874244778</v>
+        <v>218996395</v>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Samuel Chaney</t>
+          <t>Karen Wright</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>2024-03-27</t>
+          <t>2008-12-01</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>Todd Henderson</t>
+          <t>Kristina Johnston</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>465075697</v>
+        <v>394925196</v>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Douglas Hernandez</t>
+          <t>Mary Spencer</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>2012-01-18</t>
+          <t>2014-11-16</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>Nancy Jones</t>
+          <t>Danielle Ayers</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>749445940</v>
+        <v>499391405</v>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Rebecca Bailey</t>
+          <t>Joel Reid</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>2006-03-26</t>
+          <t>2014-01-31</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>Evan Calderon</t>
+          <t>Courtney Alvarado</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>186082925</v>
+        <v>598585134</v>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Jane Carter</t>
+          <t>Ashley Harris</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>2007-06-12</t>
+          <t>2018-03-09</t>
         </is>
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>Maria Thomas</t>
+          <t>Anna Thomas</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>641031533</v>
+        <v>589576488</v>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Christopher Bell</t>
+          <t>Shawn Barnes</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>2020-01-03</t>
+          <t>2010-12-14</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>Crystal Logan</t>
+          <t>Rachel Gomez</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>610140973</v>
+        <v>682562652</v>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Michelle Bradley</t>
+          <t>Kristina Lawson</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>2010-01-20</t>
+          <t>2017-05-09</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>Alan Jones</t>
+          <t>John Moore</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>830846707</v>
+        <v>412173850</v>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Christopher Francis</t>
+          <t>Kimberly Moran</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>2021-01-02</t>
+          <t>2018-10-06</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>Matthew Matthews</t>
+          <t>Heidi Aguilar</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>358726059</v>
+        <v>441816080</v>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Kevin Stafford</t>
+          <t>Christopher Gonzales</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>2024-08-07</t>
+          <t>2009-01-11</t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>Michelle Newton</t>
+          <t>Patricia Vasquez</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>293593259</v>
+        <v>856480807</v>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Victor Moore</t>
+          <t>Mandy Hall</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>2017-10-04</t>
+          <t>2008-04-24</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>Michael Bailey</t>
+          <t>Luis Shaw</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>325065952</v>
+        <v>663495386</v>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Sarah Bender</t>
+          <t>Brittney Tate</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>2006-04-17</t>
+          <t>2018-11-09</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>Tammy Diaz</t>
+          <t>Michael White</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>387429449</v>
+        <v>300056929</v>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>James Nguyen</t>
+          <t>Gina Bryant</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>2023-12-08</t>
+          <t>2009-03-14</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>Vanessa Black</t>
+          <t>Tony Johnson</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>62793420</v>
+        <v>619801546</v>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Anthony Shields</t>
+          <t>David Stuart</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>2015-11-11</t>
+          <t>2008-04-19</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>Brian Martinez</t>
+          <t>Christopher Anderson</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>38349133</v>
+        <v>520152474</v>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Taylor Vaughn</t>
+          <t>Thomas Anderson</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>2022-11-17</t>
+          <t>2017-05-04</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>Kimberly Campbell</t>
+          <t>Stephanie Fernandez</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>783008579</v>
+        <v>331288276</v>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>William Salas</t>
+          <t>Amber Mata</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>2017-10-13</t>
+          <t>2023-01-25</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>Jessica Harris</t>
+          <t>Leslie Ramirez</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>131330869</v>
+        <v>535493461</v>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Bill Flowers</t>
+          <t>Faith Murphy</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>2008-07-22</t>
+          <t>2012-02-05</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>Carl Ewing</t>
+          <t>Lisa Nichols</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>418580791</v>
+        <v>742716326</v>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Christopher Stewart</t>
+          <t>Eric Nguyen</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>2008-11-21</t>
+          <t>2021-03-16</t>
         </is>
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>Brittany Knox</t>
+          <t>Victoria Scott</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
-        <v>565162940</v>
+        <v>303629282</v>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Matthew Duarte</t>
+          <t>Samantha Hernandez</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>2023-05-09</t>
+          <t>2010-05-21</t>
         </is>
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>David Collins</t>
+          <t>Katrina Soto</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="n">
-        <v>824803972</v>
+        <v>18290156</v>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>George Lee</t>
+          <t>Stacy Moreno</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>2007-07-11</t>
+          <t>2022-01-24</t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>Alexander Allen</t>
+          <t>Joseph Davis</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>897929370</v>
+        <v>784821562</v>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Michael Lambert</t>
+          <t>Roy Long</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>2014-09-25</t>
+          <t>2018-02-12</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>Jeffrey Floyd</t>
+          <t>Scott White</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="n">
-        <v>101028688</v>
+        <v>158616245</v>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Wanda Grant</t>
+          <t>Karen Logan</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>2010-02-02</t>
+          <t>2018-11-29</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>Ann Ramirez</t>
+          <t>Brenda West</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>675772706</v>
+        <v>496023504</v>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Brianna Blankenship</t>
+          <t>Emily Ferguson</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>2022-06-12</t>
+          <t>2006-11-04</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>Elizabeth Barnett</t>
+          <t>Alexander Allen</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>86543675</v>
+        <v>931976138</v>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Stephanie Castaneda</t>
+          <t>Anne Jackson</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>2023-08-24</t>
+          <t>2010-02-20</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>Scott Wood</t>
+          <t>Melissa Wilson</t>
         </is>
       </c>
     </row>

</xml_diff>